<commit_message>
[Change] Supplier - QuerySS - 調整匯出Excel格式
</commit_message>
<xml_diff>
--- a/Platform/Platform.WebSite/ModuleResources/Other/Supplier/供應商資料匯出範本(採購).xlsx
+++ b/Platform/Platform.WebSite/ModuleResources/Other/Supplier/供應商資料匯出範本(採購).xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\加鑫科技\1.1 客戶報價單\新竹_TET\供應商平台&amp;評鑑\系統開發\Dev(供應商平台_開發)\Platform\Platform.WebSite\ModuleResources\Other\Supplier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\加鑫科技\1.1 客戶報價單\新竹_TET\供應商平台&amp;評鑑\系統開發\Dev(供應商平台&amp;評鑑_開發)\Platform\Platform.WebSite\ModuleResources\Other\Supplier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579BC139-0175-4DCA-97EE-210C279851A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9360EDB-6712-4242-9074-6E0373655568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9CCFBBE6-BC22-49C3-84C8-F09A8799A7EF}"/>
   </bookViews>
   <sheets>
     <sheet name="供應商資料" sheetId="1" r:id="rId1"/>
     <sheet name="供應商聯絡人" sheetId="2" r:id="rId2"/>
+    <sheet name="供應商STQA資訊" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>廠商類別
 Supplier Category</t>
@@ -296,28 +297,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>供應商STQA資訊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>供應商交易資訊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>供應商狀態
-Supplier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t xml:space="preserve"> Status</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -377,12 +357,17 @@
 Supplier Parent Company</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>供應商狀態
+Supplier Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -417,13 +402,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="華康中黑體"/>
-      <family val="3"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="細明體"/>
       <family val="3"/>
       <charset val="136"/>
     </font>
@@ -803,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AC91742-CCA7-4F0A-A44A-A37494EA795C}">
-  <dimension ref="A1:AY7"/>
+  <dimension ref="A1:AR7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -845,14 +823,10 @@
     <col min="40" max="40" width="29.88671875" customWidth="1"/>
     <col min="41" max="41" width="29.77734375" customWidth="1"/>
     <col min="42" max="43" width="22" customWidth="1"/>
-    <col min="44" max="44" width="12" customWidth="1"/>
-    <col min="45" max="45" width="15.5546875" customWidth="1"/>
-    <col min="46" max="46" width="14.77734375" customWidth="1"/>
-    <col min="47" max="49" width="12.109375" customWidth="1"/>
-    <col min="51" max="51" width="34.109375" customWidth="1"/>
+    <col min="44" max="44" width="34.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>52</v>
       </c>
@@ -902,31 +876,22 @@
       <c r="AO1" s="5"/>
       <c r="AP1" s="5"/>
       <c r="AQ1" s="3"/>
-      <c r="AR1" s="5" t="s">
+      <c r="AR1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AS1" s="5"/>
-      <c r="AT1" s="5"/>
-      <c r="AU1" s="5"/>
-      <c r="AV1" s="5"/>
-      <c r="AW1" s="5"/>
-      <c r="AX1" s="5"/>
-      <c r="AY1" s="3" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="2" spans="1:51" ht="90" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" ht="90" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>0</v>
@@ -1040,45 +1005,23 @@
         <v>43</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AQ2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AV2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AW2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AY2" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="AY7" s="2"/>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AR7" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:Z1"/>
     <mergeCell ref="AA1:AK1"/>
     <mergeCell ref="AL1:AP1"/>
-    <mergeCell ref="AR1:AX1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1090,7 +1033,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1131,4 +1074,58 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3614D517-203B-466D-ACBB-24BD0BB3D260}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="8" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>